<commit_message>
fix remaining bugs, exclude DG Kurve and Results. Model Runs, but is infeasible
</commit_message>
<xml_diff>
--- a/model/model_inputs_testing.xlsx
+++ b/model/model_inputs_testing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jakob\PycharmProjects\Model-1\model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{576A7F43-A542-4F64-BB55-AE29F3D4AA0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD49DA15-CB2B-4A30-B55F-A6318B5919D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="345" yWindow="345" windowWidth="14550" windowHeight="7950" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="parameters" sheetId="1" r:id="rId1"/>
@@ -1016,8 +1016,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -2488,7 +2488,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -2646,7 +2646,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC45D110-F0D2-4F9D-B0C4-13B38005F879}">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
fix bugs, delete comments, merge back to main
</commit_message>
<xml_diff>
--- a/model/model_inputs_testing.xlsx
+++ b/model/model_inputs_testing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jakob\PycharmProjects\Model-1\model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD49DA15-CB2B-4A30-B55F-A6318B5919D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFBB80BA-4737-4199-9A93-43B3004B2F50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="345" yWindow="345" windowWidth="14550" windowHeight="7950" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="parameters" sheetId="1" r:id="rId1"/>
@@ -1016,8 +1016,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -2487,7 +2487,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{254CDF95-CF95-4796-ABE1-012E5312AEC2}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -2647,7 +2647,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -2882,6 +2882,7 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
fix index from retiremend constraints, still unbounded
</commit_message>
<xml_diff>
--- a/model/model_inputs_testing.xlsx
+++ b/model/model_inputs_testing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jakob\PycharmProjects\Model-1\model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFBB80BA-4737-4199-9A93-43B3004B2F50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{825FF7A8-AEA6-401F-BC68-C12618947711}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14303" yWindow="-98" windowWidth="19394" windowHeight="10395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="parameters" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="55">
   <si>
     <t>min SoC</t>
   </si>
@@ -207,6 +207,9 @@
   </si>
   <si>
     <t>PV Rent</t>
+  </si>
+  <si>
+    <t>Unmet demand penalty</t>
   </si>
 </sst>
 </file>
@@ -1014,10 +1017,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -1028,7 +1031,7 @@
     <col min="4" max="4" width="14.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1047,8 +1050,11 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="G1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" s="1">
         <v>0.2</v>
       </c>
@@ -1066,6 +1072,9 @@
       </c>
       <c r="F2" s="1">
         <v>24</v>
+      </c>
+      <c r="G2" s="1">
+        <v>5.0000000000000001E-3</v>
       </c>
     </row>
   </sheetData>
@@ -2487,7 +2496,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{254CDF95-CF95-4796-ABE1-012E5312AEC2}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
model solveable (yay), changed 3 essential things: disp only for techs_g, revenue without battery, rented pv == prosumers capacity
</commit_message>
<xml_diff>
--- a/model/model_inputs_testing.xlsx
+++ b/model/model_inputs_testing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jakob\PycharmProjects\Model-1\model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{825FF7A8-AEA6-401F-BC68-C12618947711}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{981734DD-F5C8-44CE-A3D1-D139D6206ADA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14303" yWindow="-98" windowWidth="19394" windowHeight="10395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14303" yWindow="-98" windowWidth="19394" windowHeight="10395" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="parameters" sheetId="1" r:id="rId1"/>
@@ -1019,8 +1019,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -1074,7 +1074,7 @@
         <v>24</v>
       </c>
       <c r="G2" s="1">
-        <v>5.0000000000000001E-3</v>
+        <v>0.25</v>
       </c>
     </row>
   </sheetData>
@@ -2416,7 +2416,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -2477,10 +2477,10 @@
         <v>15</v>
       </c>
       <c r="D3" s="1">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="E3" s="1">
-        <v>300</v>
+        <v>50</v>
       </c>
       <c r="F3" s="1">
         <v>0</v>
@@ -2496,8 +2496,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{254CDF95-CF95-4796-ABE1-012E5312AEC2}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -3331,7 +3331,7 @@
   <dimension ref="A1:Y31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25"/>

</xml_diff>

<commit_message>
implement case 2: feedIn surplus (rentpv in extra branch)
</commit_message>
<xml_diff>
--- a/model/model_inputs_testing.xlsx
+++ b/model/model_inputs_testing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jakob\PycharmProjects\Model-1\model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD3C2754-9E0F-48C8-95EE-9C7101A459B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{580FE00E-2FAC-4F1E-B577-0062B630B806}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14303" yWindow="-98" windowWidth="19394" windowHeight="10395" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14303" yWindow="-98" windowWidth="19394" windowHeight="10395" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="parameters" sheetId="1" r:id="rId1"/>
@@ -111,9 +111,6 @@
     <t>Owned PV</t>
   </si>
   <si>
-    <t>Rented PV</t>
-  </si>
-  <si>
     <t>Owned Batteries</t>
   </si>
   <si>
@@ -211,6 +208,9 @@
   </si>
   <si>
     <t>Unmet demand penalty</t>
+  </si>
+  <si>
+    <t>Feed In Prosumers</t>
   </si>
 </sst>
 </file>
@@ -1021,7 +1021,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -1052,7 +1052,7 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -1172,7 +1172,7 @@
     </row>
     <row r="2" spans="1:25">
       <c r="A2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B2" s="3">
         <v>0.5</v>
@@ -1249,7 +1249,7 @@
     </row>
     <row r="3" spans="1:25">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B3" s="4">
         <v>0.5</v>
@@ -1326,7 +1326,7 @@
     </row>
     <row r="4" spans="1:25">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B4" s="4">
         <v>0.5</v>
@@ -1615,7 +1615,7 @@
     </row>
     <row r="2" spans="1:25">
       <c r="A2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B2" s="3">
         <v>0.5</v>
@@ -1692,7 +1692,7 @@
     </row>
     <row r="3" spans="1:25">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B3" s="4">
         <v>0.5</v>
@@ -1769,7 +1769,7 @@
     </row>
     <row r="4" spans="1:25">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B4" s="4">
         <v>0.5</v>
@@ -2058,7 +2058,7 @@
     </row>
     <row r="2" spans="1:25">
       <c r="A2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B2" s="3">
         <v>0.5</v>
@@ -2135,7 +2135,7 @@
     </row>
     <row r="3" spans="1:25">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B3" s="4">
         <v>0.5</v>
@@ -2212,7 +2212,7 @@
     </row>
     <row r="4" spans="1:25">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B4" s="4">
         <v>0.5</v>
@@ -2501,7 +2501,7 @@
     </row>
     <row r="2" spans="1:25">
       <c r="A2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B2" s="3">
         <v>0.5</v>
@@ -2578,7 +2578,7 @@
     </row>
     <row r="3" spans="1:25">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B3" s="4">
         <v>0.5</v>
@@ -2655,7 +2655,7 @@
     </row>
     <row r="4" spans="1:25">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B4" s="4">
         <v>0.5</v>
@@ -2859,8 +2859,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E688FB98-37F3-4971-B4CD-1E6A7262204F}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -3023,7 +3023,7 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>54</v>
       </c>
       <c r="B4" s="1">
         <v>0</v>
@@ -3046,7 +3046,7 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B5" s="1">
         <v>10</v>
@@ -3069,7 +3069,7 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B6" s="1">
         <v>20</v>
@@ -3113,18 +3113,18 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="B1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" t="s">
         <v>24</v>
       </c>
-      <c r="C1" t="s">
-        <v>25</v>
-      </c>
       <c r="D1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B2" s="1">
         <v>1.06</v>
@@ -3138,7 +3138,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B3" s="1">
         <v>1.07</v>
@@ -3152,7 +3152,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B4" s="1">
         <v>1.08</v>
@@ -3166,7 +3166,7 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B5" s="1">
         <v>1.0900000000000001</v>
@@ -3180,7 +3180,7 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B6" s="1">
         <v>1.1000000000000001</v>
@@ -3194,7 +3194,7 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B7" s="1">
         <v>1.1100000000000001</v>
@@ -3208,7 +3208,7 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B8" s="1">
         <v>1.1200000000000001</v>
@@ -3222,7 +3222,7 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B9" s="1">
         <v>1.1299999999999999</v>
@@ -3236,7 +3236,7 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B10" s="1">
         <v>1.1399999999999999</v>
@@ -3250,7 +3250,7 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B11" s="1">
         <v>1.1499999999999999</v>
@@ -3264,7 +3264,7 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B12" s="1">
         <v>1.1599999999999999</v>
@@ -3278,7 +3278,7 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B13" s="1">
         <v>1.17</v>
@@ -3292,7 +3292,7 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B14" s="1">
         <v>1.18</v>
@@ -3306,7 +3306,7 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B15" s="1">
         <v>1.19</v>
@@ -3320,7 +3320,7 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B16" s="1">
         <v>1.2</v>
@@ -3356,12 +3356,12 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="B1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B2">
         <f>(-0.2129*(0.25^3+0^3) +0.6056*(0.25^2+0^2) - 0.5538*(0.25+0) + 0.4067*2)/2</f>
@@ -3373,7 +3373,7 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B3">
         <f>(-0.2129*(0.75^3+0.25^3) +0.6056*(0.75^2+0.25^2) - 0.5538*(0.75+0.25) + 0.4067*2)/2</f>
@@ -3385,7 +3385,7 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B4">
         <f>(-0.2129*(0.75^3+0.5^3) +0.6056*(0.75^2+0.5^2) - 0.5538*(0.75+0.5) + 0.4067*2)/2</f>
@@ -3397,7 +3397,7 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B5">
         <f>(-0.2129*(1^3+0.75^3) +0.6056*(1^2+0.75^2) - 0.5538*(1+0.75) + 0.4067*2)/2</f>
@@ -3459,7 +3459,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DB9A018-F4D8-4049-8785-D914448B1EBA}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
@@ -3467,12 +3467,12 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="B1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B2" s="1">
         <v>91</v>
@@ -3480,7 +3480,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B3" s="1">
         <v>183</v>
@@ -3488,7 +3488,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B4" s="1">
         <v>91</v>
@@ -3590,7 +3590,7 @@
     </row>
     <row r="2" spans="1:25">
       <c r="A2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B2" s="1">
         <v>0</v>
@@ -3667,7 +3667,7 @@
     </row>
     <row r="3" spans="1:25">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B3" s="1">
         <v>0</v>
@@ -3744,7 +3744,7 @@
     </row>
     <row r="4" spans="1:25">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B4" s="1">
         <v>0</v>
@@ -3829,8 +3829,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ABED9F3-A079-4BB6-8141-C898B88CBE8C}">
   <dimension ref="A1:Y31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="T2" sqref="T2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -3914,7 +3914,7 @@
     </row>
     <row r="2" spans="1:25">
       <c r="A2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B2" s="3">
         <v>0.5</v>
@@ -3991,7 +3991,7 @@
     </row>
     <row r="3" spans="1:25">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B3" s="4">
         <v>0.5</v>
@@ -4068,7 +4068,7 @@
     </row>
     <row r="4" spans="1:25">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B4" s="4">
         <v>0.5</v>

</xml_diff>